<commit_message>
manage status order and manage stock
</commit_message>
<xml_diff>
--- a/public/uploads/importProductExcel.xlsx
+++ b/public/uploads/importProductExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\lavarel 8\shop-vincent\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C436A5-01C7-47FA-A81C-57BB181DA8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C74E50-2171-4611-B9D6-0CF9DE6D6EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0C7C9920-B710-474A-838A-920B6B19F826}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Game Feign</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>feign.png</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -165,8 +168,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC081EB7-7A95-4DB9-9331-7EF15E8CD643}" name="Table1" displayName="Table1" ref="A1:J20" totalsRowShown="0">
-  <autoFilter ref="A1:J20" xr:uid="{FC081EB7-7A95-4DB9-9331-7EF15E8CD643}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC081EB7-7A95-4DB9-9331-7EF15E8CD643}" name="Table1" displayName="Table1" ref="A1:K20" totalsRowShown="0">
+  <autoFilter ref="A1:K20" xr:uid="{FC081EB7-7A95-4DB9-9331-7EF15E8CD643}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -177,8 +180,9 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
     <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{45020B49-FB12-4DB7-8E76-590F00A7B87E}" name="category"/>
     <tableColumn id="2" xr3:uid="{9D1FFD06-4511-474A-A0DF-AC3F51538485}" name="brand"/>
     <tableColumn id="3" xr3:uid="{FF6A5A3E-5B87-4BB1-A8BC-4252581CF486}" name="title"/>
@@ -188,7 +192,8 @@
     <tableColumn id="7" xr3:uid="{B93F7627-D48D-404B-8C6B-B1A4B159E842}" name="content"/>
     <tableColumn id="8" xr3:uid="{D8CDBD63-07E1-4C38-896F-81CCB145DA42}" name="price"/>
     <tableColumn id="9" xr3:uid="{5B1CAC2F-36AD-4530-9D58-452413B2A36D}" name="image"/>
-    <tableColumn id="10" xr3:uid="{A664D625-019A-4EAA-BF6F-EE28CBA5B77D}" name="status"/>
+    <tableColumn id="12" xr3:uid="{5C6895A3-16E8-45E3-8C89-E7804D2C4224}" name="status"/>
+    <tableColumn id="10" xr3:uid="{A664D625-019A-4EAA-BF6F-EE28CBA5B77D}" name="quantity"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -491,19 +496,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2507FEFA-260F-4B91-8AEE-6332A1C52095}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="10.09765625" customWidth="1"/>
-    <col min="10" max="10" width="11.09765625" customWidth="1"/>
+    <col min="1" max="10" width="10.09765625" customWidth="1"/>
+    <col min="11" max="11" width="11.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -534,8 +539,11 @@
       <c r="J1" t="s">
         <v>14</v>
       </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>8</v>
       </c>
@@ -565,6 +573,9 @@
       </c>
       <c r="J2" s="1">
         <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>